<commit_message>
Fixed x2 mini35 BoM.
</commit_message>
<xml_diff>
--- a/cam/LED-mini35-SHIM_x2_2021-09-03-BoM.xlsx
+++ b/cam/LED-mini35-SHIM_x2_2021-09-03-BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\LED-SHIM\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F51796B-BD18-42B8-AC49-0FB50FAE6A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21B6D74-0C46-4D9C-9A7C-54158D451790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21620" yWindow="620" windowWidth="17320" windowHeight="19950" xr2:uid="{87EF1620-7AD1-4553-BDCE-AB53403D6CB9}"/>
+    <workbookView xWindow="1140" yWindow="1050" windowWidth="17320" windowHeight="19950" xr2:uid="{87EF1620-7AD1-4553-BDCE-AB53403D6CB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,10 +95,10 @@
     <t>C1, C2, C3, C4</t>
   </si>
   <si>
-    <t>IC1, IC3</t>
-  </si>
-  <si>
     <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9, LED10, LED11, LED12, LED13, LED14, LED15, LED16, LED17, LED18, LED19, LED20, LED21, LED22, LED23, LED24</t>
+  </si>
+  <si>
+    <t>IC1, IC2</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,7 +556,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
@@ -590,10 +590,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -610,7 +610,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>

</xml_diff>